<commit_message>
tum veriler cekiliyor yalniz excele header yazmiyor
</commit_message>
<xml_diff>
--- a/New_Excel.xlsx
+++ b/New_Excel.xlsx
@@ -389,11 +389,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -402,11 +402,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -415,11 +415,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -428,11 +428,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6">
@@ -441,11 +441,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -454,11 +454,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -467,11 +467,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -480,11 +480,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -493,11 +493,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
@@ -506,11 +506,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -519,11 +519,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2020-05-06 18:20</t>
+          <t>2020-05-09 16:47</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>